<commit_message>
Added the full project
</commit_message>
<xml_diff>
--- a/DummyAutomation/TestConfigsData/TestData.xlsx
+++ b/DummyAutomation/TestConfigsData/TestData.xlsx
@@ -12,7 +12,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -31,13 +30,13 @@
     <t>SelectOptionNumber</t>
   </si>
   <si>
-    <t>Ipad</t>
-  </si>
-  <si>
     <t>TC-02</t>
   </si>
   <si>
-    <t>Cover</t>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>IPAD</t>
   </si>
 </sst>
 </file>
@@ -379,7 +378,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,7 +404,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -413,10 +412,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
       </c>
       <c r="C3">
         <v>2</v>

</xml_diff>